<commit_message>
agrega campo Activo a tabla Usuarios
</commit_message>
<xml_diff>
--- a/ModeloSQL/DatosConsultoria.xlsx
+++ b/ModeloSQL/DatosConsultoria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\takes\Dropbox\Awakelab\M4JavaWeb\ModeloSQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Awakelab\M4JavaWeb\ModeloSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7018B865-EC85-4F49-B18C-27438EA0A144}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FC1A40-093F-4B9F-90DB-B78F438625C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="2490" windowWidth="20490" windowHeight="10920" firstSheet="7" activeTab="9" xr2:uid="{511FF998-9EBB-47D5-872C-28D19E21C3B0}"/>
+    <workbookView xWindow="58815" yWindow="300" windowWidth="27675" windowHeight="14985" activeTab="8" xr2:uid="{511FF998-9EBB-47D5-872C-28D19E21C3B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuario" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,22 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="173">
-  <si>
-    <t>idusuario</t>
-  </si>
-  <si>
-    <t>usuario</t>
-  </si>
-  <si>
-    <t>tipousuario</t>
-  </si>
-  <si>
-    <t>clave</t>
-  </si>
-  <si>
-    <t>mail</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="174">
   <si>
     <t>admin1</t>
   </si>
@@ -564,6 +547,24 @@
   </si>
   <si>
     <t>TOTALES</t>
+  </si>
+  <si>
+    <t>IDUSUARIO</t>
+  </si>
+  <si>
+    <t>USUARIO</t>
+  </si>
+  <si>
+    <t>TIPOUSUARIO</t>
+  </si>
+  <si>
+    <t>CLAVE</t>
+  </si>
+  <si>
+    <t>MAIL</t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
   </si>
 </sst>
 </file>
@@ -924,10 +925,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CB9A35-960F-4587-8E85-7B3822F70B51}">
-  <dimension ref="A1:E11"/>
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A7"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -938,32 +942,35 @@
     <col min="5" max="5" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>123</v>
@@ -972,16 +979,19 @@
         <f>_xlfn.CONCAT(B2,"@consultoria.cl")</f>
         <v>admin1@consultoria.cl</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>123</v>
@@ -990,16 +1000,19 @@
         <f t="shared" ref="E3:E11" si="0">_xlfn.CONCAT(B3,"@consultoria.cl")</f>
         <v>admin2@consultoria.cl</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4">
         <v>123</v>
@@ -1008,16 +1021,19 @@
         <f>_xlfn.CONCAT(B4,"@",B4,".com")</f>
         <v>cliente1@cliente1.com</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D5">
         <v>123</v>
@@ -1026,16 +1042,19 @@
         <f t="shared" ref="E5:E7" si="1">_xlfn.CONCAT(B5,"@",B5,".com")</f>
         <v>cliente2@cliente2.com</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>123</v>
@@ -1044,16 +1063,19 @@
         <f t="shared" si="1"/>
         <v>cliente3@cliente3.com</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7">
         <v>123</v>
@@ -1062,16 +1084,19 @@
         <f t="shared" si="1"/>
         <v>cliente4@cliente4.com</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D8">
         <v>123</v>
@@ -1080,16 +1105,19 @@
         <f t="shared" si="0"/>
         <v>prev1@consultoria.cl</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>123</v>
@@ -1098,16 +1126,19 @@
         <f t="shared" si="0"/>
         <v>prev2@consultoria.cl</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>123</v>
@@ -1116,16 +1147,19 @@
         <f t="shared" si="0"/>
         <v>prev3@consultoria.cl</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <v>123</v>
@@ -1133,6 +1167,9 @@
       <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>prev4@consultoria.cl</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1144,10 +1181,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C435395A-7C62-4729-9AC0-1BFEBB7B6371}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="A2:E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,19 +1199,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1179,7 +1219,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C2" s="1">
         <v>1000</v>
@@ -1196,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1">
         <v>1000</v>
@@ -1213,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1">
         <v>1000</v>
@@ -1230,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C5" s="1">
         <v>1000</v>
@@ -1247,7 +1287,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C6" s="1">
         <v>1000</v>
@@ -1264,7 +1304,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C7" s="1">
         <v>100</v>
@@ -1281,7 +1321,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C8" s="1">
         <v>1000</v>
@@ -1298,7 +1338,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C9" s="1">
         <v>100</v>
@@ -1310,10 +1350,10 @@
         <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="H9" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="I9">
         <v>1</v>
@@ -1324,7 +1364,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C10" s="1">
         <v>10</v>
@@ -1336,10 +1376,10 @@
         <v>6</v>
       </c>
       <c r="G10" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" t="s">
         <v>157</v>
-      </c>
-      <c r="H10" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1347,7 +1387,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C11" s="1">
         <v>1000</v>
@@ -1359,10 +1399,10 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="H11" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1370,7 +1410,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C12" s="1">
         <v>100</v>
@@ -1382,10 +1422,10 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="H12" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1393,7 +1433,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C13" s="1">
         <v>700</v>
@@ -1410,7 +1450,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C14" s="1">
         <v>1000</v>
@@ -1427,7 +1467,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C15" s="1">
         <v>100</v>
@@ -1444,7 +1484,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C16" s="1">
         <v>700</v>
@@ -1461,7 +1501,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C17" s="1">
         <v>1000</v>
@@ -1478,7 +1518,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C18" s="1">
         <v>1000</v>
@@ -1495,7 +1535,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C19" s="1">
         <v>100</v>
@@ -1512,7 +1552,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C20" s="1">
         <v>10</v>
@@ -1529,7 +1569,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C21" s="1">
         <v>1000</v>
@@ -1546,7 +1586,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C22" s="1">
         <v>10</v>
@@ -1563,7 +1603,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C23" s="1">
         <v>1000</v>
@@ -1580,7 +1620,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C24" s="1">
         <v>500</v>
@@ -1597,7 +1637,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C25" s="1">
         <v>1000</v>
@@ -1614,7 +1654,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C26" s="1">
         <v>100</v>
@@ -1631,7 +1671,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C27" s="1">
         <v>10</v>
@@ -1648,7 +1688,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C28" s="1">
         <v>1000</v>
@@ -1665,7 +1705,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C29" s="1">
         <v>500</v>
@@ -1682,7 +1722,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C30" s="1">
         <v>700</v>
@@ -1699,7 +1739,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C31" s="1">
         <v>10</v>
@@ -1720,6 +1760,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB0493B-8F99-4561-A7FE-9A6C17F47C7D}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1736,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C1">
         <v>1</v>
@@ -1747,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1761,6 +1804,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD9C6FB-6030-4530-A9C2-9EFF9A624256}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1775,16 +1821,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1792,13 +1838,13 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1806,13 +1852,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1820,13 +1866,13 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C4">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1834,13 +1880,13 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1851,6 +1897,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C69C56-7699-4E68-95CA-ECD640CAC8A5}">
+  <sheetPr>
+    <tabColor theme="7"/>
+  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1866,16 +1915,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1883,7 +1932,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2">
         <v>76000001</v>
@@ -1897,7 +1946,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C3">
         <v>76000002</v>
@@ -1911,7 +1960,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C4">
         <v>76000003</v>
@@ -1925,7 +1974,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C5">
         <v>76000004</v>
@@ -1942,6 +1991,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517B7494-F2BE-402B-88A1-808A76BA52EF}">
+  <sheetPr>
+    <tabColor rgb="FF7030A0"/>
+  </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1960,25 +2012,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" t="s">
+      <c r="G1" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1986,19 +2038,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2009,19 +2061,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -2032,19 +2084,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
         <v>47</v>
       </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" t="s">
-        <v>52</v>
-      </c>
       <c r="F4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -2055,19 +2107,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2078,19 +2130,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2101,19 +2153,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>20</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -2124,19 +2176,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -2147,19 +2199,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>30</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -2170,19 +2222,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2193,19 +2245,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -2216,19 +2268,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>20</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -2239,19 +2291,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C13">
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="F13" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G13">
         <v>4</v>
@@ -2262,19 +2314,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -2285,19 +2337,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -2318,6 +2370,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67B7D32-7CD8-4C8C-B812-B9FCC66DE30A}">
+  <sheetPr>
+    <tabColor theme="5" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2334,19 +2389,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2354,13 +2409,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2371,13 +2426,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2388,13 +2443,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -2405,13 +2460,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -2425,6 +2480,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F2E691-C1ED-43C6-9189-DE5EEBCED1AB}">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2444,25 +2502,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2470,19 +2528,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D2" s="2">
         <v>43952</v>
       </c>
       <c r="E2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -2493,19 +2551,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2">
         <v>43984</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G3">
         <v>2</v>
@@ -2516,19 +2574,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D4" s="2">
         <v>44046</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G4">
         <v>3</v>
@@ -2539,19 +2597,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2">
         <v>44108</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G5">
         <v>4</v>
@@ -2562,19 +2620,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2">
         <v>44170</v>
       </c>
       <c r="E6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -2585,19 +2643,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2">
         <v>44141</v>
       </c>
       <c r="E7" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -2608,19 +2666,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2">
         <v>43928</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="G8">
         <v>3</v>
@@ -2631,19 +2689,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D9" s="2">
         <v>43898</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -2654,19 +2712,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D10" s="2">
         <v>44113</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -2677,19 +2735,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D11" s="2">
         <v>44084</v>
       </c>
       <c r="E11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -2700,19 +2758,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C12" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="D12" s="2">
         <v>44115</v>
       </c>
       <c r="E12" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F12" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -2755,28 +2813,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2787,16 +2845,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G2" s="2">
         <v>43952</v>
@@ -2813,16 +2871,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D3" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G3" s="2">
         <v>43984</v>
@@ -2839,16 +2897,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G4" s="2">
         <v>44046</v>
@@ -2865,16 +2923,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G5" s="2">
         <v>44108</v>
@@ -2891,16 +2949,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D6" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="G6" s="2">
         <v>44170</v>
@@ -2917,16 +2975,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F7" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G7" s="2">
         <v>44141</v>
@@ -2943,16 +3001,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D8" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F8" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G8" s="2">
         <v>43928</v>
@@ -2969,16 +3027,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G9" s="2">
         <v>43898</v>
@@ -2995,16 +3053,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D10" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F10" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G10" s="2">
         <v>44113</v>
@@ -3021,16 +3079,16 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F11" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G11" s="2">
         <v>44084</v>
@@ -3047,16 +3105,16 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="F12" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G12" s="2">
         <v>44115</v>
@@ -3073,9 +3131,12 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3912E3C0-2835-4B06-8161-90CF3B925B8D}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H15" sqref="A2:H15"/>
     </sheetView>
   </sheetViews>
@@ -3092,28 +3153,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
         <v>166</v>
       </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
         <v>167</v>
-      </c>
-      <c r="D1" t="s">
-        <v>168</v>
-      </c>
-      <c r="E1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" t="s">
-        <v>170</v>
-      </c>
-      <c r="G1" t="s">
-        <v>171</v>
-      </c>
-      <c r="H1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -3127,7 +3188,7 @@
         <v>43891</v>
       </c>
       <c r="D2" s="2">
-        <f>+C2+30</f>
+        <f t="shared" ref="D2:D13" si="0">+C2+30</f>
         <v>43921</v>
       </c>
       <c r="E2" s="2">
@@ -3148,7 +3209,7 @@
         <v>43891</v>
       </c>
       <c r="D3" s="2">
-        <f>+C3+30</f>
+        <f t="shared" si="0"/>
         <v>43921</v>
       </c>
       <c r="E3" s="2">
@@ -3169,7 +3230,7 @@
         <v>43891</v>
       </c>
       <c r="D4" s="2">
-        <f>+C4+30</f>
+        <f t="shared" si="0"/>
         <v>43921</v>
       </c>
       <c r="E4" s="2">
@@ -3190,7 +3251,7 @@
         <v>43891</v>
       </c>
       <c r="D5" s="2">
-        <f>+C5+30</f>
+        <f t="shared" si="0"/>
         <v>43921</v>
       </c>
       <c r="E5" s="2">
@@ -3211,7 +3272,7 @@
         <v>43922</v>
       </c>
       <c r="D6" s="2">
-        <f>+C6+30</f>
+        <f t="shared" si="0"/>
         <v>43952</v>
       </c>
       <c r="E6" s="2">
@@ -3232,7 +3293,7 @@
         <v>43922</v>
       </c>
       <c r="D7" s="2">
-        <f>+C7+30</f>
+        <f t="shared" si="0"/>
         <v>43952</v>
       </c>
       <c r="E7" s="2">
@@ -3253,7 +3314,7 @@
         <v>43922</v>
       </c>
       <c r="D8" s="2">
-        <f>+C8+30</f>
+        <f t="shared" si="0"/>
         <v>43952</v>
       </c>
       <c r="E8" s="2">
@@ -3274,7 +3335,7 @@
         <v>43922</v>
       </c>
       <c r="D9" s="2">
-        <f>+C9+30</f>
+        <f t="shared" si="0"/>
         <v>43952</v>
       </c>
       <c r="E9" s="2">
@@ -3295,7 +3356,7 @@
         <v>43952</v>
       </c>
       <c r="D10" s="2">
-        <f>+C10+30</f>
+        <f t="shared" si="0"/>
         <v>43982</v>
       </c>
       <c r="F10" s="1">
@@ -3313,7 +3374,7 @@
         <v>43952</v>
       </c>
       <c r="D11" s="2">
-        <f>+C11+30</f>
+        <f t="shared" si="0"/>
         <v>43982</v>
       </c>
       <c r="F11" s="1">
@@ -3331,7 +3392,7 @@
         <v>43952</v>
       </c>
       <c r="D12" s="2">
-        <f>+C12+30</f>
+        <f t="shared" si="0"/>
         <v>43982</v>
       </c>
       <c r="F12" s="1">
@@ -3349,7 +3410,7 @@
         <v>43952</v>
       </c>
       <c r="D13" s="2">
-        <f>+C13+30</f>
+        <f t="shared" si="0"/>
         <v>43982</v>
       </c>
       <c r="F13" s="1">
@@ -3367,7 +3428,7 @@
         <v>43983</v>
       </c>
       <c r="D14" s="2">
-        <f t="shared" ref="D14:D15" si="0">+C14+30</f>
+        <f t="shared" ref="D14" si="1">+C14+30</f>
         <v>44013</v>
       </c>
       <c r="F14" s="1">

</xml_diff>

<commit_message>
ahora si que si
</commit_message>
<xml_diff>
--- a/ModeloSQL/DatosConsultoria.xlsx
+++ b/ModeloSQL/DatosConsultoria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Awakelab\M4JavaWeb\ModeloSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FC1A40-093F-4B9F-90DB-B78F438625C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C819D905-01B2-4836-9AA3-FA713007073F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58815" yWindow="300" windowWidth="27675" windowHeight="14985" activeTab="8" xr2:uid="{511FF998-9EBB-47D5-872C-28D19E21C3B0}"/>
+    <workbookView xWindow="58725" yWindow="300" windowWidth="27675" windowHeight="14985" activeTab="9" xr2:uid="{511FF998-9EBB-47D5-872C-28D19E21C3B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuario" sheetId="1" r:id="rId1"/>
@@ -42,8 +42,112 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={34BD564E-4144-4B74-83BF-2CD718397830}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{34BD564E-4144-4B74-83BF-2CD718397830}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    autoincrement</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Takeshi Kita</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{467F7DBF-3DD4-4EC7-B578-BED278FCDE33}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Takeshi Kita:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+autoincrement</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Takeshi Kita</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{E4D5CC80-CEEF-4650-8E7B-0468E1CD7084}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Takeshi Kita:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+autoincrement</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={33B2F2DC-AB80-450A-82E6-CB14DD7454E6}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{33B2F2DC-AB80-450A-82E6-CB14DD7454E6}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    autoincrement</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="176">
   <si>
     <t>admin1</t>
   </si>
@@ -565,13 +669,19 @@
   </si>
   <si>
     <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>IDEMPLEADO</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,6 +694,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -606,11 +742,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,6 +765,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Takeshi Kita" id="{B123450E-B29C-446A-A855-159136D3973E}" userId="52184c335830e1f8" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -923,19 +1068,36 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2020-07-01T22:34:48.68" personId="{B123450E-B29C-446A-A855-159136D3973E}" id="{34BD564E-4144-4B74-83BF-2CD718397830}">
+    <text>autoincrement</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2020-07-01T22:35:05.80" personId="{B123450E-B29C-446A-A855-159136D3973E}" id="{33B2F2DC-AB80-450A-82E6-CB14DD7454E6}">
+    <text>autoincrement</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CB9A35-960F-4587-8E85-7B3822F70B51}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CB9A35-960F-4587-8E85-7B3822F70B51}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="F11" sqref="B2:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
@@ -943,7 +1105,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B1" t="s">
@@ -963,7 +1125,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -984,7 +1146,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1005,7 +1167,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1026,7 +1188,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1047,7 +1209,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1068,7 +1230,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1089,7 +1251,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1110,7 +1272,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1131,7 +1293,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1152,7 +1314,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1176,6 +1338,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1186,19 +1349,20 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="B2:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B1" t="s">
@@ -1215,7 +1379,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1232,7 +1396,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1249,7 +1413,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1266,7 +1430,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1283,7 +1447,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -1300,7 +1464,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -1317,7 +1481,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -1334,7 +1498,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -1360,7 +1524,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -1383,7 +1547,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -1406,7 +1570,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -1429,7 +1593,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -1446,7 +1610,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -1463,7 +1627,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -1480,7 +1644,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -1497,7 +1661,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -1514,7 +1678,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -1531,7 +1695,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -1548,7 +1712,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="4">
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -1565,7 +1729,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -1582,7 +1746,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -1599,7 +1763,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -1616,7 +1780,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -1633,7 +1797,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -1650,7 +1814,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -1667,7 +1831,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -1684,7 +1848,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
       <c r="B28" t="s">
@@ -1701,7 +1865,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
       <c r="B29" t="s">
@@ -1718,7 +1882,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
       <c r="B30" t="s">
@@ -1735,7 +1899,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
       <c r="B31" t="s">
@@ -1763,36 +1927,49 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C3" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2">
+      <c r="C3" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1903,18 +2080,19 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D5"/>
+      <selection activeCell="D5" sqref="B2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
     <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B1" t="s">
@@ -1928,7 +2106,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1942,7 +2120,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1956,7 +2134,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1970,7 +2148,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -1990,28 +2168,29 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517B7494-F2BE-402B-88A1-808A76BA52EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517B7494-F2BE-402B-88A1-808A76BA52EF}">
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+      <selection activeCell="B2" sqref="B2:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
@@ -2034,7 +2213,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -2057,7 +2236,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -2080,7 +2259,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -2103,7 +2282,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -2126,7 +2305,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -2149,7 +2328,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -2172,7 +2351,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -2195,7 +2374,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -2218,7 +2397,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -2241,7 +2420,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -2264,7 +2443,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -2287,7 +2466,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -2310,7 +2489,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -2333,7 +2512,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -2365,6 +2544,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2376,19 +2556,20 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E5" sqref="B2:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
       <c r="B1" t="s">
@@ -2405,7 +2586,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -2422,7 +2603,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2439,7 +2620,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -2456,7 +2637,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -2479,19 +2660,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F2E691-C1ED-43C6-9189-DE5EEBCED1AB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F2E691-C1ED-43C6-9189-DE5EEBCED1AB}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B2" sqref="B2:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
     <col min="3" max="3" width="45.140625" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
@@ -2501,7 +2682,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>90</v>
       </c>
       <c r="B1" t="s">
@@ -2524,7 +2705,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -2547,7 +2728,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -2570,7 +2751,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -2593,7 +2774,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -2616,7 +2797,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -2639,7 +2820,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -2662,7 +2843,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -2685,7 +2866,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -2708,7 +2889,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -2731,7 +2912,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -2754,7 +2935,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -2787,6 +2968,7 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2797,14 +2979,14 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="B2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="45.42578125" style="1" customWidth="1"/>
@@ -2812,11 +2994,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>120</v>
@@ -2838,7 +3020,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
@@ -2864,7 +3046,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3">
@@ -2890,7 +3072,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4">
@@ -2916,7 +3098,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5">
@@ -2942,11 +3124,11 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
+      <c r="A6" s="4">
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>126</v>
@@ -2968,11 +3150,11 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>2</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>131</v>
@@ -2994,11 +3176,11 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>3</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>134</v>
@@ -3020,11 +3202,11 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>4</v>
-      </c>
-      <c r="B9">
-        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>137</v>
@@ -3046,11 +3228,11 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
+      <c r="A10" s="4">
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>137</v>
@@ -3072,11 +3254,11 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>2</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
       </c>
       <c r="C11" t="s">
         <v>141</v>
@@ -3098,11 +3280,11 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12">
         <v>3</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
       </c>
       <c r="C12" t="s">
         <v>141</v>
@@ -3130,18 +3312,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3912E3C0-2835-4B06-8161-90CF3B925B8D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3912E3C0-2835-4B06-8161-90CF3B925B8D}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="A2:H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="B2:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
@@ -3152,7 +3335,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>161</v>
       </c>
       <c r="B1" t="s">
@@ -3178,7 +3361,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
       <c r="B2">
@@ -3199,7 +3382,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
       <c r="B3">
@@ -3220,7 +3403,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4">
@@ -3241,7 +3424,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5">
@@ -3262,7 +3445,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6">
@@ -3283,7 +3466,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7">
@@ -3304,7 +3487,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8">
@@ -3325,7 +3508,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9">
@@ -3346,7 +3529,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10">
@@ -3364,7 +3547,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11">
@@ -3382,7 +3565,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
       <c r="B12">
@@ -3400,7 +3583,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
       <c r="B13">
@@ -3418,7 +3601,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
       <c r="B14">
@@ -3436,7 +3619,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
       <c r="B15">
@@ -3456,5 +3639,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agrega Casos de asesoria
</commit_message>
<xml_diff>
--- a/ModeloSQL/DatosConsultoria.xlsx
+++ b/ModeloSQL/DatosConsultoria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Awakelab\M5JavaSpring\ModeloSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A30A663-8CCC-4590-9DFB-D43F506F0279}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC28F6C-418C-4FEE-8A1B-76133FF1E80A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="0" windowWidth="27675" windowHeight="14985" xr2:uid="{511FF998-9EBB-47D5-872C-28D19E21C3B0}"/>
+    <workbookView xWindow="29355" yWindow="315" windowWidth="27675" windowHeight="14985" firstSheet="4" activeTab="13" xr2:uid="{511FF998-9EBB-47D5-872C-28D19E21C3B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Usuario" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="Item" sheetId="9" r:id="rId10"/>
     <sheet name="Preguntas" sheetId="11" r:id="rId11"/>
     <sheet name="Checklists" sheetId="12" r:id="rId12"/>
+    <sheet name="CasoAsesoria" sheetId="13" r:id="rId13"/>
+    <sheet name="Asesoria" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Actividad!$A$1:$G$1</definedName>
@@ -151,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="306">
   <si>
     <t>admin1</t>
   </si>
@@ -991,6 +993,84 @@
   </si>
   <si>
     <t>$2a$10$/Vj4nUtV/nBonAnUZ1Ka5.3L1dhy1J6ZPF0lkJftb62CMpHsztHzi</t>
+  </si>
+  <si>
+    <t>IDCASO</t>
+  </si>
+  <si>
+    <t>CODIGOCONTRATO</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>CONTACTO</t>
+  </si>
+  <si>
+    <t>CASOACTIVO</t>
+  </si>
+  <si>
+    <t>COD-2020-0001</t>
+  </si>
+  <si>
+    <t>COD-1997-0002</t>
+  </si>
+  <si>
+    <t>COD-2019-0003</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Juan Dorado</t>
+  </si>
+  <si>
+    <t>Sofia Calipso</t>
+  </si>
+  <si>
+    <t>Pedro Blanco</t>
+  </si>
+  <si>
+    <t>IDASESORIA</t>
+  </si>
+  <si>
+    <t>CASOASESORIA_IDCASO</t>
+  </si>
+  <si>
+    <t>FECHAASESORIA</t>
+  </si>
+  <si>
+    <t>PROFESIONAL</t>
+  </si>
+  <si>
+    <t>LUGAR</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>Blanco Encalada 300</t>
+  </si>
+  <si>
+    <t>Sin hallazgos</t>
+  </si>
+  <si>
+    <t>Oficina central Calipso</t>
+  </si>
+  <si>
+    <t>Oficina regional VI Calipso</t>
+  </si>
+  <si>
+    <t>Oficina Central Dorado</t>
+  </si>
+  <si>
+    <t>Bodega Dorado</t>
+  </si>
+  <si>
+    <t>Oficina Central Blanco</t>
+  </si>
+  <si>
+    <t>Oficina Regional IV Blanco</t>
   </si>
 </sst>
 </file>
@@ -1098,6 +1178,7 @@
   <colors>
     <mruColors>
       <color rgb="FF0000FF"/>
+      <color rgb="FFFC0480"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1435,8 +1516,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,7 +2354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CF0EB33-7A2C-4853-85F9-57904AEDAF61}">
   <dimension ref="A1:E61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E61" sqref="A2:E61"/>
     </sheetView>
   </sheetViews>
@@ -3249,6 +3330,1911 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C154DD48-B47A-498B-9827-CF2E6FBCFF4C}">
+  <sheetPr>
+    <tabColor rgb="FFFC0480"/>
+  </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="2" max="2" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D1" t="s">
+        <v>282</v>
+      </c>
+      <c r="E1" t="s">
+        <v>283</v>
+      </c>
+      <c r="F1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>285</v>
+      </c>
+      <c r="D2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D3" t="s">
+        <v>288</v>
+      </c>
+      <c r="E3" t="s">
+        <v>290</v>
+      </c>
+      <c r="F3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14D49DD4-04C1-4A6A-9828-E8F6340D6778}">
+  <dimension ref="A1:G85"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="2" max="2" width="22.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C1" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F1" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43832</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>302</v>
+      </c>
+      <c r="F2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT("insert into 'casoasesoria' ( ",$B$1,") values(",E2,");")</f>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43839</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>303</v>
+      </c>
+      <c r="F3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G19" si="0">_xlfn.CONCAT("insert into 'casoasesoria' ( ",$B$1,") values(",E3,");")</f>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Bodega Dorado);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43846</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F4" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Bodega Dorado);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43853</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>302</v>
+      </c>
+      <c r="F5" t="s">
+        <v>299</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43864</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>302</v>
+      </c>
+      <c r="F6" t="s">
+        <v>299</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43877</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7" t="s">
+        <v>302</v>
+      </c>
+      <c r="F7" t="s">
+        <v>299</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43881</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>302</v>
+      </c>
+      <c r="F8" t="s">
+        <v>299</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>43886</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>302</v>
+      </c>
+      <c r="F9" t="s">
+        <v>299</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43893</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>302</v>
+      </c>
+      <c r="F10" t="s">
+        <v>299</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <v>43906</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>303</v>
+      </c>
+      <c r="F11" t="s">
+        <v>299</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Bodega Dorado);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2">
+        <v>43910</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>302</v>
+      </c>
+      <c r="F12" t="s">
+        <v>299</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>43915</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>302</v>
+      </c>
+      <c r="F13" t="s">
+        <v>299</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="8">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>43924</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>302</v>
+      </c>
+      <c r="F14" t="s">
+        <v>299</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>43937</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>302</v>
+      </c>
+      <c r="F15" t="s">
+        <v>299</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="8">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>303</v>
+      </c>
+      <c r="F16" t="s">
+        <v>299</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Bodega Dorado);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2">
+        <v>43946</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17" t="s">
+        <v>302</v>
+      </c>
+      <c r="F17" t="s">
+        <v>299</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2">
+        <v>43954</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>302</v>
+      </c>
+      <c r="F18" t="s">
+        <v>299</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>43967</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>302</v>
+      </c>
+      <c r="F19" t="s">
+        <v>299</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>insert into 'casoasesoria' ( CASOASESORIA_IDCASO) values(Oficina Central Dorado);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="8">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>43971</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>302</v>
+      </c>
+      <c r="F20" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="8">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>43976</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>302</v>
+      </c>
+      <c r="F21" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>21</v>
+      </c>
+      <c r="B22" s="8">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>43985</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>302</v>
+      </c>
+      <c r="F22" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>43998</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>302</v>
+      </c>
+      <c r="F23" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44002</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>298</v>
+      </c>
+      <c r="F24" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>24</v>
+      </c>
+      <c r="B25" s="8">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44007</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>298</v>
+      </c>
+      <c r="F25" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="8">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44015</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>298</v>
+      </c>
+      <c r="F26" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" s="8">
+        <v>1</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44028</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27" t="s">
+        <v>298</v>
+      </c>
+      <c r="F27" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>27</v>
+      </c>
+      <c r="B28" s="8">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44032</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>303</v>
+      </c>
+      <c r="F28" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>28</v>
+      </c>
+      <c r="B29" s="8">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44037</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>298</v>
+      </c>
+      <c r="F29" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>29</v>
+      </c>
+      <c r="B30" s="8">
+        <v>2</v>
+      </c>
+      <c r="C30" s="2">
+        <v>43832</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>300</v>
+      </c>
+      <c r="F30" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>30</v>
+      </c>
+      <c r="B31" s="8">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>43839</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>301</v>
+      </c>
+      <c r="F31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>31</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2</v>
+      </c>
+      <c r="C32" s="2">
+        <v>43842</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>32</v>
+      </c>
+      <c r="B33" s="8">
+        <v>2</v>
+      </c>
+      <c r="C33" s="2">
+        <v>43853</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>300</v>
+      </c>
+      <c r="F33" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>33</v>
+      </c>
+      <c r="B34" s="8">
+        <v>2</v>
+      </c>
+      <c r="C34" s="2">
+        <v>43863</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>300</v>
+      </c>
+      <c r="F34" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>34</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>43873</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>300</v>
+      </c>
+      <c r="F35" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>43881</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>300</v>
+      </c>
+      <c r="F36" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>43888</v>
+      </c>
+      <c r="D37">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>300</v>
+      </c>
+      <c r="F37" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="8">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>43896</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>300</v>
+      </c>
+      <c r="F38" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="8">
+        <v>2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>43902</v>
+      </c>
+      <c r="D39">
+        <v>5</v>
+      </c>
+      <c r="E39" t="s">
+        <v>300</v>
+      </c>
+      <c r="F39" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="8">
+        <v>2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>43910</v>
+      </c>
+      <c r="D40">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>300</v>
+      </c>
+      <c r="F40" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="8">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>43917</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>300</v>
+      </c>
+      <c r="F41" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="8">
+        <v>2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>43924</v>
+      </c>
+      <c r="D42">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>300</v>
+      </c>
+      <c r="F42" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8">
+        <v>2</v>
+      </c>
+      <c r="C43" s="2">
+        <v>43933</v>
+      </c>
+      <c r="D43">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>301</v>
+      </c>
+      <c r="F43" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>43941</v>
+      </c>
+      <c r="D44">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>301</v>
+      </c>
+      <c r="F44" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="8">
+        <v>2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>43948</v>
+      </c>
+      <c r="D45">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>301</v>
+      </c>
+      <c r="F45" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="8">
+        <v>2</v>
+      </c>
+      <c r="C46" s="2">
+        <v>43954</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="E46" t="s">
+        <v>301</v>
+      </c>
+      <c r="F46" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="8">
+        <v>2</v>
+      </c>
+      <c r="C47" s="2">
+        <v>43963</v>
+      </c>
+      <c r="D47">
+        <v>6</v>
+      </c>
+      <c r="E47" t="s">
+        <v>301</v>
+      </c>
+      <c r="F47" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="8">
+        <v>2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>43971</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>300</v>
+      </c>
+      <c r="F48" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="8">
+        <v>2</v>
+      </c>
+      <c r="C49" s="2">
+        <v>43978</v>
+      </c>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="E49" t="s">
+        <v>300</v>
+      </c>
+      <c r="F49" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
+      <c r="B50" s="8">
+        <v>2</v>
+      </c>
+      <c r="C50" s="2">
+        <v>43985</v>
+      </c>
+      <c r="D50">
+        <v>4</v>
+      </c>
+      <c r="E50" t="s">
+        <v>300</v>
+      </c>
+      <c r="F50" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
+      <c r="B51" s="8">
+        <v>2</v>
+      </c>
+      <c r="C51" s="2">
+        <v>43994</v>
+      </c>
+      <c r="D51">
+        <v>6</v>
+      </c>
+      <c r="E51" t="s">
+        <v>300</v>
+      </c>
+      <c r="F51" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
+      <c r="B52" s="8">
+        <v>2</v>
+      </c>
+      <c r="C52" s="2">
+        <v>44002</v>
+      </c>
+      <c r="D52">
+        <v>4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>300</v>
+      </c>
+      <c r="F52" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
+      <c r="B53" s="8">
+        <v>2</v>
+      </c>
+      <c r="C53" s="2">
+        <v>44009</v>
+      </c>
+      <c r="D53">
+        <v>6</v>
+      </c>
+      <c r="E53" t="s">
+        <v>300</v>
+      </c>
+      <c r="F53" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8">
+        <v>2</v>
+      </c>
+      <c r="C54" s="2">
+        <v>44015</v>
+      </c>
+      <c r="D54">
+        <v>6</v>
+      </c>
+      <c r="E54" t="s">
+        <v>300</v>
+      </c>
+      <c r="F54" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
+      <c r="B55" s="8">
+        <v>2</v>
+      </c>
+      <c r="C55" s="2">
+        <v>44024</v>
+      </c>
+      <c r="D55">
+        <v>6</v>
+      </c>
+      <c r="E55" t="s">
+        <v>300</v>
+      </c>
+      <c r="F55" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
+      <c r="B56" s="8">
+        <v>2</v>
+      </c>
+      <c r="C56" s="2">
+        <v>44032</v>
+      </c>
+      <c r="D56">
+        <v>6</v>
+      </c>
+      <c r="E56" t="s">
+        <v>300</v>
+      </c>
+      <c r="F56" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
+      <c r="B57" s="8">
+        <v>2</v>
+      </c>
+      <c r="C57" s="2">
+        <v>44039</v>
+      </c>
+      <c r="D57">
+        <v>6</v>
+      </c>
+      <c r="E57" t="s">
+        <v>301</v>
+      </c>
+      <c r="F57" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
+      <c r="B58" s="8">
+        <v>3</v>
+      </c>
+      <c r="C58" s="2">
+        <v>43832</v>
+      </c>
+      <c r="D58">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>304</v>
+      </c>
+      <c r="F58" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
+      <c r="B59" s="8">
+        <v>3</v>
+      </c>
+      <c r="C59" s="2">
+        <v>43839</v>
+      </c>
+      <c r="D59">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
+        <v>305</v>
+      </c>
+      <c r="F59" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
+      <c r="B60" s="8">
+        <v>3</v>
+      </c>
+      <c r="C60" s="2">
+        <v>43841</v>
+      </c>
+      <c r="D60">
+        <v>5</v>
+      </c>
+      <c r="E60" t="s">
+        <v>305</v>
+      </c>
+      <c r="F60" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
+      <c r="B61" s="8">
+        <v>3</v>
+      </c>
+      <c r="C61" s="2">
+        <v>43853</v>
+      </c>
+      <c r="D61">
+        <v>5</v>
+      </c>
+      <c r="E61" t="s">
+        <v>305</v>
+      </c>
+      <c r="F61" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
+      <c r="B62" s="8">
+        <v>3</v>
+      </c>
+      <c r="C62" s="2">
+        <v>43863</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>305</v>
+      </c>
+      <c r="F62" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
+      <c r="B63" s="8">
+        <v>3</v>
+      </c>
+      <c r="C63" s="2">
+        <v>43872</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>305</v>
+      </c>
+      <c r="F63" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="4">
+        <v>63</v>
+      </c>
+      <c r="B64" s="8">
+        <v>3</v>
+      </c>
+      <c r="C64" s="2">
+        <v>43881</v>
+      </c>
+      <c r="D64">
+        <v>5</v>
+      </c>
+      <c r="E64" t="s">
+        <v>305</v>
+      </c>
+      <c r="F64" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="4">
+        <v>64</v>
+      </c>
+      <c r="B65" s="8">
+        <v>3</v>
+      </c>
+      <c r="C65" s="2">
+        <v>43889</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>304</v>
+      </c>
+      <c r="F65" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
+      <c r="B66" s="8">
+        <v>3</v>
+      </c>
+      <c r="C66" s="2">
+        <v>43896</v>
+      </c>
+      <c r="D66">
+        <v>5</v>
+      </c>
+      <c r="E66" t="s">
+        <v>305</v>
+      </c>
+      <c r="F66" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="4">
+        <v>66</v>
+      </c>
+      <c r="B67" s="8">
+        <v>3</v>
+      </c>
+      <c r="C67" s="2">
+        <v>43901</v>
+      </c>
+      <c r="D67">
+        <v>5</v>
+      </c>
+      <c r="E67" t="s">
+        <v>305</v>
+      </c>
+      <c r="F67" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>67</v>
+      </c>
+      <c r="B68" s="8">
+        <v>3</v>
+      </c>
+      <c r="C68" s="2">
+        <v>43910</v>
+      </c>
+      <c r="D68">
+        <v>5</v>
+      </c>
+      <c r="E68" t="s">
+        <v>305</v>
+      </c>
+      <c r="F68" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>68</v>
+      </c>
+      <c r="B69" s="8">
+        <v>3</v>
+      </c>
+      <c r="C69" s="2">
+        <v>43918</v>
+      </c>
+      <c r="D69">
+        <v>5</v>
+      </c>
+      <c r="E69" t="s">
+        <v>305</v>
+      </c>
+      <c r="F69" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>69</v>
+      </c>
+      <c r="B70" s="8">
+        <v>3</v>
+      </c>
+      <c r="C70" s="2">
+        <v>43924</v>
+      </c>
+      <c r="D70">
+        <v>5</v>
+      </c>
+      <c r="E70" t="s">
+        <v>305</v>
+      </c>
+      <c r="F70" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>70</v>
+      </c>
+      <c r="B71" s="8">
+        <v>3</v>
+      </c>
+      <c r="C71" s="2">
+        <v>43932</v>
+      </c>
+      <c r="D71">
+        <v>5</v>
+      </c>
+      <c r="E71" t="s">
+        <v>305</v>
+      </c>
+      <c r="F71" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>71</v>
+      </c>
+      <c r="B72" s="8">
+        <v>3</v>
+      </c>
+      <c r="C72" s="2">
+        <v>43946</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>305</v>
+      </c>
+      <c r="F72" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>72</v>
+      </c>
+      <c r="B73" s="8">
+        <v>3</v>
+      </c>
+      <c r="C73" s="2">
+        <v>43949</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>304</v>
+      </c>
+      <c r="F73" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>73</v>
+      </c>
+      <c r="B74" s="8">
+        <v>3</v>
+      </c>
+      <c r="C74" s="2">
+        <v>43954</v>
+      </c>
+      <c r="D74">
+        <v>5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>304</v>
+      </c>
+      <c r="F74" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>74</v>
+      </c>
+      <c r="B75" s="8">
+        <v>3</v>
+      </c>
+      <c r="C75" s="2">
+        <v>43962</v>
+      </c>
+      <c r="D75">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>304</v>
+      </c>
+      <c r="F75" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>75</v>
+      </c>
+      <c r="B76" s="8">
+        <v>3</v>
+      </c>
+      <c r="C76" s="2">
+        <v>43970</v>
+      </c>
+      <c r="D76">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>304</v>
+      </c>
+      <c r="F76" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>76</v>
+      </c>
+      <c r="B77" s="8">
+        <v>3</v>
+      </c>
+      <c r="C77" s="2">
+        <v>43979</v>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>304</v>
+      </c>
+      <c r="F77" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>77</v>
+      </c>
+      <c r="B78" s="8">
+        <v>3</v>
+      </c>
+      <c r="C78" s="2">
+        <v>43985</v>
+      </c>
+      <c r="D78">
+        <v>5</v>
+      </c>
+      <c r="E78" t="s">
+        <v>304</v>
+      </c>
+      <c r="F78" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>78</v>
+      </c>
+      <c r="B79" s="8">
+        <v>3</v>
+      </c>
+      <c r="C79" s="2">
+        <v>43993</v>
+      </c>
+      <c r="D79">
+        <v>5</v>
+      </c>
+      <c r="E79" t="s">
+        <v>305</v>
+      </c>
+      <c r="F79" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="4">
+        <v>79</v>
+      </c>
+      <c r="B80" s="8">
+        <v>3</v>
+      </c>
+      <c r="C80" s="2">
+        <v>44002</v>
+      </c>
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80" t="s">
+        <v>305</v>
+      </c>
+      <c r="F80" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>80</v>
+      </c>
+      <c r="B81" s="8">
+        <v>3</v>
+      </c>
+      <c r="C81" s="2">
+        <v>44010</v>
+      </c>
+      <c r="D81">
+        <v>5</v>
+      </c>
+      <c r="E81" t="s">
+        <v>305</v>
+      </c>
+      <c r="F81" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>81</v>
+      </c>
+      <c r="B82" s="8">
+        <v>3</v>
+      </c>
+      <c r="C82" s="2">
+        <v>44015</v>
+      </c>
+      <c r="D82">
+        <v>5</v>
+      </c>
+      <c r="E82" t="s">
+        <v>305</v>
+      </c>
+      <c r="F82" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>82</v>
+      </c>
+      <c r="B83" s="8">
+        <v>3</v>
+      </c>
+      <c r="C83" s="2">
+        <v>44023</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83" t="s">
+        <v>305</v>
+      </c>
+      <c r="F83" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>83</v>
+      </c>
+      <c r="B84" s="8">
+        <v>3</v>
+      </c>
+      <c r="C84" s="2">
+        <v>44032</v>
+      </c>
+      <c r="D84">
+        <v>6</v>
+      </c>
+      <c r="E84" t="s">
+        <v>305</v>
+      </c>
+      <c r="F84" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>84</v>
+      </c>
+      <c r="B85" s="8">
+        <v>3</v>
+      </c>
+      <c r="C85" s="2">
+        <v>44040</v>
+      </c>
+      <c r="D85">
+        <v>5</v>
+      </c>
+      <c r="E85" t="s">
+        <v>304</v>
+      </c>
+      <c r="F85" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4367,7 +6353,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="B2:H12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4706,7 +6692,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="B2:F15"/>
+      <selection activeCell="C5" sqref="C5:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>